<commit_message>
New test cases: Execution time VS Number of scores
</commit_message>
<xml_diff>
--- a/reports/results.xlsx
+++ b/reports/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\mnapps\DominanceQueries\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEF0D987-AC91-40FD-BB92-85AB2C9C569B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D76F0CF-7FBD-4C79-896B-40A84282C279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E19CD79E-1BA2-4C91-BDB9-2094BB8A9E62}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E19CD79E-1BA2-4C91-BDB9-2094BB8A9E62}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Distribution</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Uniform</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -2351,6 +2354,1618 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="el-GR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution time per number of cores</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>[Anti-Correlated, 1M Sampes, 3 Dimensions]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="el-GR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Get top 10 Skyline Points</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$E$22:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$K$22:$K$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43.666200000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.819000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.118120000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F713-464B-BA7C-C53D19A3B59C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1855946655"/>
+        <c:axId val="1855950815"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1855946655"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cores</a:t>
+                </a:r>
+                <a:endParaRPr lang="el-GR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="el-GR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1855950815"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1855950815"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Seconds</a:t>
+                </a:r>
+                <a:endParaRPr lang="el-GR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="el-GR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1855946655"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="el-GR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="el-GR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="el-GR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution time per number of cores</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>[Anti-Correlated, 1M Sampes, 3 Dimensions]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="el-GR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Get top 10 points</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$E$22:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$J$22:$J$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>843.91520000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>644.976</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>604.92679999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-12ED-41A5-890B-7960BE16974A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="95665535"/>
+        <c:axId val="95670527"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="95665535"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95670527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="95670527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="95665535"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="el-GR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="el-GR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="el-GR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution time per number of cores</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>[Anti-Correlated, 1M Sampes, 3 Dimensions]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="el-GR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Get skyline points</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$E$22:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$I$22:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>35.476869999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36.376199999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.896299999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1961-4937-B080-77C1A7A04356}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="433098863"/>
+        <c:axId val="433101359"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="433098863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433101359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="433101359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433098863"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="el-GR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="el-GR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="el-GR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Execution time per number of cores</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>[Anti-Correlated, 1M Sampes, 3 Dimensions]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="el-GR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Gather and sort data</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Results!$E$22:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Results!$H$22:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6.2888999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.2553000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8982999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7692-40D8-A737-2E84887F9AF6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="433094287"/>
+        <c:axId val="433081807"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="433094287"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433081807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="433081807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="el-GR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="433094287"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="el-GR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="el-GR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2471,6 +4086,166 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3987,6 +5762,2070 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4117,6 +7956,158 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>484094</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>116541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>179294</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>170329</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Γράφημα 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C412A92-D4C7-407F-A060-7EFA79E3F901}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>349624</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>44824</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>35859</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Γράφημα 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6A4F221-4CFD-484A-875C-D4C383802F41}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>98612</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161365</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>35859</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Γράφημα 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A3B95EC2-F59D-4364-B9E6-ED30E65848AD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>546846</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>242046</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>8965</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Γράφημα 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B297A287-FDE5-4A3B-8175-6BD0D788FC34}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4424,8 +8415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DBEA462-3014-44F4-8051-ACB2DBCDFE38}">
   <dimension ref="B3:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H22" activeCellId="1" sqref="E22:E24 H22:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5056,28 +9047,100 @@
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C22" s="1"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H22" s="2">
+        <v>6.2888999999999999</v>
+      </c>
+      <c r="I22" s="2">
+        <v>35.476869999999998</v>
+      </c>
+      <c r="J22" s="2">
+        <v>843.91520000000003</v>
+      </c>
+      <c r="K22" s="2">
+        <v>43.666200000000003</v>
+      </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C23" s="1"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
+      <c r="B23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="2">
+        <v>5.2553000000000001</v>
+      </c>
+      <c r="I23" s="2">
+        <v>36.376199999999997</v>
+      </c>
+      <c r="J23" s="2">
+        <v>644.976</v>
+      </c>
+      <c r="K23" s="2">
+        <v>36.819000000000003</v>
+      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="C24" s="1"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1">
+        <v>100</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H24" s="2">
+        <v>4.8982999999999999</v>
+      </c>
+      <c r="I24" s="2">
+        <v>33.896299999999997</v>
+      </c>
+      <c r="J24" s="2">
+        <v>604.92679999999996</v>
+      </c>
+      <c r="K24" s="2">
+        <v>30.118120000000001</v>
+      </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.3">
       <c r="C25" s="1"/>
@@ -5120,8 +9183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5623001-6ADE-41EB-B4F5-86692CD838B8}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="K19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>